<commit_message>
update using latest pdf of ieee students
</commit_message>
<xml_diff>
--- a/IEEESBAwardChecklist.xlsx
+++ b/IEEESBAwardChecklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ikostelidis\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8A1040F-3C6B-4100-9896-0EFADD6BC150}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{762C91B9-FF56-48D5-A305-2EAD1671BFA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Φύλλο1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -78,9 +81,6 @@
     <t>Fund raisers</t>
   </si>
   <si>
-    <t>Hosting an SPAC</t>
-  </si>
-  <si>
     <t>Must of Required</t>
   </si>
   <si>
@@ -117,12 +117,6 @@
     <t>Entry in the Region Hardware Design Contest</t>
   </si>
   <si>
-    <t>Participation in the Student Enterprise Award</t>
-  </si>
-  <si>
-    <t>Organizing an S-PAVe</t>
-  </si>
-  <si>
     <t>Nomination for Larry K. Wilson Regional Student Activities Award</t>
   </si>
   <si>
@@ -144,9 +138,6 @@
     <t>Formation of a new SB Chapter / Affinity Group</t>
   </si>
   <si>
-    <t>Other SB Activities</t>
-  </si>
-  <si>
     <t>Technical workshops</t>
   </si>
   <si>
@@ -157,6 +148,18 @@
   </si>
   <si>
     <t>We Earn It?</t>
+  </si>
+  <si>
+    <t>Hosting a Student Professional Awareness Conference</t>
+  </si>
+  <si>
+    <t>Student Branch participation in IEEE Student Competitions such as IEEEXtreme, IEEEmadC, etc.</t>
+  </si>
+  <si>
+    <t>Participation of Student Branch Members in Humanitarian Activities</t>
+  </si>
+  <si>
+    <t>Upload Additional Documentation about Student Branch Activities (Optional)</t>
   </si>
 </sst>
 </file>
@@ -523,14 +526,14 @@
   <dimension ref="A1:W1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="B6" sqref="B2:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="38.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="61.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="84.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.85546875" bestFit="1" customWidth="1"/>
@@ -733,7 +736,7 @@
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="3" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
@@ -758,14 +761,14 @@
     </row>
     <row r="8" spans="1:23" ht="12.75">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="6">
         <f>COUNTA(A2:A6)</f>
         <v>5</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
@@ -790,14 +793,14 @@
     </row>
     <row r="9" spans="1:23" ht="14.25">
       <c r="A9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" s="7">
         <f>COUNTA(B2:B6)</f>
         <v>0</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="4"/>
@@ -822,14 +825,14 @@
     </row>
     <row r="10" spans="1:23" ht="12.75">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="6" t="str">
         <f>IF((B9&gt;=B8),"YES","NO")</f>
         <v>NO</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="4"/>
@@ -856,7 +859,7 @@
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="4"/>
@@ -883,7 +886,7 @@
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="4"/>
@@ -910,7 +913,7 @@
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="4"/>
@@ -937,7 +940,7 @@
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="4"/>
@@ -964,7 +967,7 @@
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
@@ -991,7 +994,7 @@
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
@@ -1017,8 +1020,8 @@
     <row r="17" spans="1:23" ht="12.75">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
-      <c r="C17" s="3" t="s">
-        <v>29</v>
+      <c r="C17" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
@@ -1044,8 +1047,8 @@
     <row r="18" spans="1:23" ht="12.75">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
-      <c r="C18" s="3" t="s">
-        <v>30</v>
+      <c r="C18" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
@@ -1072,7 +1075,7 @@
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
@@ -1099,7 +1102,7 @@
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
@@ -1126,7 +1129,7 @@
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
@@ -1153,7 +1156,7 @@
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
@@ -1180,7 +1183,7 @@
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="4"/>
@@ -1207,7 +1210,7 @@
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="4"/>
@@ -1234,7 +1237,7 @@
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
@@ -1261,7 +1264,7 @@
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="4"/>
@@ -1288,7 +1291,7 @@
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="4"/>
@@ -1315,9 +1318,9 @@
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
-      <c r="D28" s="3"/>
+      <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
@@ -1341,8 +1344,8 @@
     <row r="29" spans="1:23" ht="12.75">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
-      <c r="C29" s="3" t="s">
-        <v>41</v>
+      <c r="C29" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
@@ -1373,7 +1376,7 @@
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
       <c r="G30" s="8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="H30" s="9" t="str">
         <f>IF(AND(F3="YES",B10="YES"),"YES","NO")</f>
@@ -1395,7 +1398,7 @@
       <c r="V30" s="4"/>
       <c r="W30" s="4"/>
     </row>
-    <row r="31" spans="1:23">
+    <row r="31" spans="1:23" ht="12.75">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -1420,7 +1423,7 @@
       <c r="V31" s="4"/>
       <c r="W31" s="4"/>
     </row>
-    <row r="32" spans="1:23">
+    <row r="32" spans="1:23" ht="12.75">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -1445,7 +1448,7 @@
       <c r="V32" s="4"/>
       <c r="W32" s="4"/>
     </row>
-    <row r="33" spans="1:23">
+    <row r="33" spans="1:23" ht="12.75">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -1470,7 +1473,7 @@
       <c r="V33" s="4"/>
       <c r="W33" s="4"/>
     </row>
-    <row r="34" spans="1:23">
+    <row r="34" spans="1:23" ht="12.75">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -1495,7 +1498,7 @@
       <c r="V34" s="4"/>
       <c r="W34" s="4"/>
     </row>
-    <row r="35" spans="1:23">
+    <row r="35" spans="1:23" ht="12.75">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -1520,7 +1523,7 @@
       <c r="V35" s="4"/>
       <c r="W35" s="4"/>
     </row>
-    <row r="36" spans="1:23">
+    <row r="36" spans="1:23" ht="12.75">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -1545,7 +1548,7 @@
       <c r="V36" s="4"/>
       <c r="W36" s="4"/>
     </row>
-    <row r="37" spans="1:23">
+    <row r="37" spans="1:23" ht="12.75">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>

</xml_diff>

<commit_message>
update title of additional 1
</commit_message>
<xml_diff>
--- a/IEEESBAwardChecklist.xlsx
+++ b/IEEESBAwardChecklist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ikostelidis\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ikostelidis\ExcelProjects\IEEESBAwardChecklist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{762C91B9-FF56-48D5-A305-2EAD1671BFA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64C8F01A-66D2-47AD-BF7A-D37F510DD1E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2250" yWindow="2250" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Φύλλο1" sheetId="1" r:id="rId1"/>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>Student Branch Online Activity Report</t>
-  </si>
-  <si>
-    <t>Application for Awards</t>
   </si>
   <si>
     <t>Additional We Have</t>
@@ -160,6 +157,9 @@
   </si>
   <si>
     <t>Upload Additional Documentation about Student Branch Activities (Optional)</t>
+  </si>
+  <si>
+    <t>Application copy of one of the IEEE Awards &amp; Scholarship Programs</t>
   </si>
 </sst>
 </file>
@@ -526,7 +526,7 @@
   <dimension ref="A1:W1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B2:B6"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -583,11 +583,11 @@
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F2" s="5">
         <f>COUNTA(D2:D29)</f>
@@ -613,15 +613,15 @@
     </row>
     <row r="3" spans="1:23" ht="12.75">
       <c r="A3" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" s="6" t="str">
         <f>IF((F2&gt;=F1),"YES","NO")</f>
@@ -647,11 +647,11 @@
     </row>
     <row r="4" spans="1:23" ht="12.75">
       <c r="A4" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="4"/>
@@ -676,11 +676,11 @@
     </row>
     <row r="5" spans="1:23" ht="12.75">
       <c r="A5" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="4"/>
@@ -705,11 +705,11 @@
     </row>
     <row r="6" spans="1:23" ht="12.75">
       <c r="A6" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -736,7 +736,7 @@
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
@@ -761,14 +761,14 @@
     </row>
     <row r="8" spans="1:23" ht="12.75">
       <c r="A8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="6">
         <f>COUNTA(A2:A6)</f>
         <v>5</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
@@ -793,14 +793,14 @@
     </row>
     <row r="9" spans="1:23" ht="14.25">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="7">
         <f>COUNTA(B2:B6)</f>
         <v>0</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="4"/>
@@ -825,14 +825,14 @@
     </row>
     <row r="10" spans="1:23" ht="12.75">
       <c r="A10" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="6" t="str">
         <f>IF((B9&gt;=B8),"YES","NO")</f>
         <v>NO</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="4"/>
@@ -859,7 +859,7 @@
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="4"/>
@@ -886,7 +886,7 @@
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="4"/>
@@ -913,7 +913,7 @@
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="4"/>
@@ -940,7 +940,7 @@
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="4"/>
@@ -967,7 +967,7 @@
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
@@ -994,7 +994,7 @@
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
@@ -1021,7 +1021,7 @@
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
@@ -1048,7 +1048,7 @@
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
@@ -1075,7 +1075,7 @@
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
@@ -1102,7 +1102,7 @@
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
@@ -1129,7 +1129,7 @@
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
@@ -1156,7 +1156,7 @@
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
@@ -1183,7 +1183,7 @@
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="4"/>
@@ -1210,7 +1210,7 @@
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="4"/>
@@ -1237,7 +1237,7 @@
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
@@ -1264,7 +1264,7 @@
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="4"/>
@@ -1291,7 +1291,7 @@
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="4"/>
@@ -1318,7 +1318,7 @@
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
@@ -1345,7 +1345,7 @@
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
@@ -1376,7 +1376,7 @@
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
       <c r="G30" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H30" s="9" t="str">
         <f>IF(AND(F3="YES",B10="YES"),"YES","NO")</f>

</xml_diff>